<commit_message>
Removed localized fields in account group (Build 452)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint24Plan.xlsx
+++ b/doc/Planning/Sprint24Plan.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -170,6 +170,21 @@
   </si>
   <si>
     <t>تکمیل امکانات موجود</t>
+  </si>
+  <si>
+    <t>مدیریت اطلاعات گروه های حساب</t>
+  </si>
+  <si>
+    <t>پیاده سازی عملیات اصلی مدیریت گروه های حساب در سرویس وب</t>
+  </si>
+  <si>
+    <t>مدیریت اطلاعات گروه های حساب در برنامه وب</t>
+  </si>
+  <si>
+    <t>اضافه کردن شناسه گروه حساب برای حساب های کل در سرویس وب</t>
+  </si>
+  <si>
+    <t>امکان انتخاب گروه حساب هنگام ایجاد و اصلاح حساب های کل در برنامه وب</t>
   </si>
 </sst>
 </file>
@@ -1038,8 +1053,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E25" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
-  <autoFilter ref="A2:E25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E29" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
+  <autoFilter ref="A2:E29"/>
   <tableColumns count="5">
     <tableColumn id="1" name="هدف کاری" dataDxfId="43"/>
     <tableColumn id="2" name="قابلیت" dataDxfId="42"/>
@@ -1371,10 +1386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1491,10 +1506,10 @@
     </row>
     <row r="10" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1505,7 +1520,7 @@
     <row r="11" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
@@ -1516,7 +1531,7 @@
     <row r="12" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -1527,7 +1542,7 @@
     <row r="13" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -1536,9 +1551,11 @@
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="B14" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -1549,7 +1566,7 @@
     <row r="15" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -1560,7 +1577,7 @@
     <row r="16" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -1571,7 +1588,7 @@
     <row r="17" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -1582,7 +1599,7 @@
     <row r="18" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
@@ -1591,11 +1608,9 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="A19" s="7"/>
       <c r="B19" s="4" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -1606,7 +1621,7 @@
     <row r="20" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -1617,59 +1632,105 @@
     <row r="21" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>39</v>
-      </c>
+      <c r="D21" s="5"/>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="D22" s="5"/>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
+      <c r="A23" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="B23" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="D23" s="5"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13:C17 C3:C10 C20:C25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C17:C21 C3:C14 C24:C29">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Voucher standard form with details in Report API (Build 457)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint24Plan.xlsx
+++ b/doc/Planning/Sprint24Plan.xlsx
@@ -94,36 +94,9 @@
     <t>امکان انتخاب حساب با توجه به ارتباطات موجود در کنترل حساب - مشابه رفتار موجود در پوسته وب جدید</t>
   </si>
   <si>
-    <t>آماده کردن اطلاعات گزارش مدیریت اسناد در سرویس وب</t>
-  </si>
-  <si>
-    <t>نمایش گزارش مدیریت اسناد در برنامه با امکان پیش نمایش و چاپ</t>
-  </si>
-  <si>
-    <t>طراحی قالب نمایشی گزارش مدیریت اسناد در محیط طراحی زیرساخت گزارشات</t>
-  </si>
-  <si>
     <t>تکمیل ساختار اطلاعاتی سند مالی و آرتیکل مالی مطابق با تحلیل موجود</t>
   </si>
   <si>
-    <t>آماده کردن اطلاعات گزارش خلاصه سند مالی در سرویس وب</t>
-  </si>
-  <si>
-    <t>طراحی قالب نمایشی گزارش خلاصه سند مالی</t>
-  </si>
-  <si>
-    <t>نمایش گزارش خلاصه سند مالی با امکان پیش نمایش و چاپ</t>
-  </si>
-  <si>
-    <t>آماده کردن اطلاعات گزارش چاپی سند مالی کامل در سرویس وب</t>
-  </si>
-  <si>
-    <t>طراحی قالب نمایشی گزارش چاپی سند مالی کامل</t>
-  </si>
-  <si>
-    <t>نمایش گزارش چاپی سند مالی کامل با امکان پیش نمایش و چاپ</t>
-  </si>
-  <si>
     <t>اعمال تنظیمات نمایشی اعداد مطابق با اطلاعات فرم تنظیمات در برنامه - استفاده از جداکننده</t>
   </si>
   <si>
@@ -185,6 +158,33 @@
   </si>
   <si>
     <t>امکان انتخاب گروه حساب هنگام ایجاد و اصلاح حساب های کل در برنامه وب</t>
+  </si>
+  <si>
+    <t>آماده کردن اطلاعات گزارش خلاصه اسناد در سرویس وب</t>
+  </si>
+  <si>
+    <t>نمایش گزارش خلاصه اسناد در برنامه با امکان پیش نمایش و چاپ</t>
+  </si>
+  <si>
+    <t>طراحی قالب نمایشی گزارش خلاصه اسناد در محیط طراحی زیرساخت گزارشات</t>
+  </si>
+  <si>
+    <t>آماده کردن اطلاعات گزارش فرم مرسوم سند در سرویس وب</t>
+  </si>
+  <si>
+    <t>طراحی قالب نمایشی گزارش فرم مرسوم سند</t>
+  </si>
+  <si>
+    <t>نمایش گزارش فرم مرسوم سند با امکان پیش نمایش و چاپ</t>
+  </si>
+  <si>
+    <t>طراحی قالب نمایشی گزارش چاپی سند مالی با سطوح شناور</t>
+  </si>
+  <si>
+    <t>نمایش گزارش چاپی سند مالی با سطوح شناور با امکان پیش نمایش و چاپ</t>
+  </si>
+  <si>
+    <t>آماده کردن اطلاعات گزارش چاپی سند مالی با سطوح شناور در سرویس وب</t>
   </si>
 </sst>
 </file>
@@ -1388,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1425,7 +1425,7 @@
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>18</v>
@@ -1449,10 +1449,10 @@
     </row>
     <row r="5" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -1463,7 +1463,7 @@
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -1474,7 +1474,7 @@
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -1485,7 +1485,7 @@
     <row r="8" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -1496,7 +1496,7 @@
     <row r="9" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -1506,10 +1506,10 @@
     </row>
     <row r="10" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1520,7 +1520,7 @@
     <row r="11" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
@@ -1531,7 +1531,7 @@
     <row r="12" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -1542,7 +1542,7 @@
     <row r="13" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -1552,10 +1552,10 @@
     </row>
     <row r="14" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -1566,7 +1566,7 @@
     <row r="15" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -1577,7 +1577,7 @@
     <row r="16" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -1588,7 +1588,7 @@
     <row r="17" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="4" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -1599,7 +1599,7 @@
     <row r="18" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
@@ -1610,7 +1610,7 @@
     <row r="19" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="4" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -1621,7 +1621,7 @@
     <row r="20" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="4" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -1632,7 +1632,7 @@
     <row r="21" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="4" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
@@ -1643,7 +1643,7 @@
     <row r="22" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="4" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
@@ -1653,10 +1653,10 @@
     </row>
     <row r="23" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C23" s="5">
         <v>1</v>
@@ -1667,7 +1667,7 @@
     <row r="24" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C24" s="5">
         <v>1</v>
@@ -1678,39 +1678,39 @@
     <row r="25" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C25" s="5">
         <v>1</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5">
         <v>1</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C27" s="5">
         <v>1</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E27" s="4"/>
     </row>

</xml_diff>